<commit_message>
updated shot data with Dartmouth game.
</commit_message>
<xml_diff>
--- a/brown_shots.xlsx
+++ b/brown_shots.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlie/Data/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7F9376-1BF0-6C4D-A3EF-EC37A6F8546F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C786506B-72AC-8C43-AF88-4FDEF2645F37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="460" windowWidth="16620" windowHeight="11960" xr2:uid="{E7FACA18-4C05-B649-B97D-C07BF93FF78E}"/>
+    <workbookView xWindow="8940" yWindow="460" windowWidth="13720" windowHeight="11960" xr2:uid="{E7FACA18-4C05-B649-B97D-C07BF93FF78E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="28">
   <si>
     <t>sh_num</t>
   </si>
@@ -106,6 +111,9 @@
   </si>
   <si>
     <t>#26- N. Andrews</t>
+  </si>
+  <si>
+    <t>Defensive Midfield</t>
   </si>
 </sst>
 </file>
@@ -459,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEC312E-ABDF-E24A-B5B9-9C6AB014BA4C}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,7 +623,7 @@
         <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated with Cornell and Penn data.
</commit_message>
<xml_diff>
--- a/brown_shots.xlsx
+++ b/brown_shots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlie/Data/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C786506B-72AC-8C43-AF88-4FDEF2645F37}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56D8AC8-3B83-284E-9B0D-1F8AD238D3B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8940" yWindow="460" windowWidth="13720" windowHeight="11960" xr2:uid="{E7FACA18-4C05-B649-B97D-C07BF93FF78E}"/>
   </bookViews>
@@ -98,22 +98,22 @@
     <t>F</t>
   </si>
   <si>
-    <t>#35- W. Cheek</t>
-  </si>
-  <si>
-    <t>#48- K. Salvatore</t>
-  </si>
-  <si>
-    <t>#9- S. Evans</t>
-  </si>
-  <si>
-    <t>#24- J. Lang</t>
-  </si>
-  <si>
-    <t>#26- N. Andrews</t>
-  </si>
-  <si>
     <t>Defensive Midfield</t>
+  </si>
+  <si>
+    <t>#35 - W. Cheek</t>
+  </si>
+  <si>
+    <t>#48 - K. Salvatore</t>
+  </si>
+  <si>
+    <t>#9 - S. Evans</t>
+  </si>
+  <si>
+    <t>#24 - J. Lang</t>
+  </si>
+  <si>
+    <t>#26 - N. Andrews</t>
   </si>
 </sst>
 </file>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FEC312E-ABDF-E24A-B5B9-9C6AB014BA4C}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,7 +623,7 @@
         <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I11" t="s">
         <v>14</v>
@@ -899,7 +899,7 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
@@ -992,7 +992,7 @@
         <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I17" t="s">
         <v>14</v>
@@ -1054,7 +1054,7 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I19" t="s">
         <v>14</v>
@@ -1178,7 +1178,7 @@
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I23" t="s">
         <v>9</v>
@@ -1209,7 +1209,7 @@
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I24" t="s">
         <v>9</v>
@@ -1302,7 +1302,7 @@
         <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I27" t="s">
         <v>14</v>

</xml_diff>